<commit_message>
use 190506 version Ear benchmark report
</commit_message>
<xml_diff>
--- a/lib/report/benchmark_report/web14/exl/201812/jsliu__bank_test_&_city_(HF)(201812)_EaR.xlsx
+++ b/lib/report/benchmark_report/web14/exl/201812/jsliu__bank_test_&_city_(HF)(201812)_EaR.xlsx
@@ -567,7 +567,7 @@
     <t xml:space="preserve">Portfolio Name : jsliu  bank test &amp; city (HF)-201812</t>
   </si>
   <si>
-    <t xml:space="preserve">As of 12/31/18    Printed on: 04/03/19 12:47:42 PM</t>
+    <t xml:space="preserve">As of 12/31/18    Printed on: 05/06/19 4:52:52 AM</t>
   </si>
   <si>
     <t>1/31/2019</t>
@@ -67927,7 +67927,7 @@
         <v>6</v>
       </c>
       <c r="K11" s="274">
-        <v>2.6925028</v>
+        <v>2.69711309</v>
       </c>
       <c r="L11" s="274">
         <v>0</v>
@@ -67936,7 +67936,7 @@
         <v>0</v>
       </c>
       <c r="N11" s="274">
-        <v>0.30962079</v>
+        <v>0.30549964</v>
       </c>
       <c r="O11" s="277" t="s">
         <v>182</v>
@@ -67971,7 +67971,7 @@
         <v>6</v>
       </c>
       <c r="K12" s="274">
-        <v>2.69251407</v>
+        <v>2.69712373</v>
       </c>
       <c r="L12" s="274">
         <v>0</v>
@@ -67980,7 +67980,7 @@
         <v>0</v>
       </c>
       <c r="N12" s="274">
-        <v>0.30813651</v>
+        <v>0.30444192000000003</v>
       </c>
       <c r="O12" s="277" t="s">
         <v>184</v>
@@ -68053,16 +68053,16 @@
         <v>75</v>
       </c>
       <c r="K15" s="274">
-        <v>2.76264743</v>
+        <v>2.7640732000000003</v>
       </c>
       <c r="L15" s="274">
-        <v>0.0887621</v>
+        <v>0.08870172</v>
       </c>
       <c r="M15" s="274">
-        <v>0.24814306</v>
+        <v>0.17481586000000002</v>
       </c>
       <c r="N15" s="274">
-        <v>-0.07419979</v>
+        <v>-0.0027535800000000003</v>
       </c>
       <c r="O15" s="277" t="s">
         <v>188</v>
@@ -68116,7 +68116,7 @@
         <v>6</v>
       </c>
       <c r="K17" s="274">
-        <v>2.67974153</v>
+        <v>2.68808975</v>
       </c>
       <c r="L17" s="274">
         <v>0</v>
@@ -68125,7 +68125,7 @@
         <v>0</v>
       </c>
       <c r="N17" s="274">
-        <v>0.31961709</v>
+        <v>0.31306686</v>
       </c>
       <c r="O17" s="277" t="s">
         <v>191</v>
@@ -68217,16 +68217,16 @@
         <v>75</v>
       </c>
       <c r="K21" s="274">
-        <v>2.4663246400000003</v>
+        <v>2.46116567</v>
       </c>
       <c r="L21" s="274">
-        <v>0.00013578</v>
+        <v>8.88E-06</v>
       </c>
       <c r="M21" s="274">
-        <v>0.49499991</v>
+        <v>0.49357078000000004</v>
       </c>
       <c r="N21" s="274">
-        <v>0.06562891</v>
+        <v>0.063999040000000007</v>
       </c>
       <c r="O21" s="277" t="s">
         <v>196</v>
@@ -68261,16 +68261,16 @@
         <v>75</v>
       </c>
       <c r="K22" s="274">
-        <v>2.4663246400000003</v>
+        <v>2.46116567</v>
       </c>
       <c r="L22" s="274">
-        <v>0.00013578</v>
+        <v>8.88E-06</v>
       </c>
       <c r="M22" s="274">
-        <v>0.49499991</v>
+        <v>0.49357078000000004</v>
       </c>
       <c r="N22" s="274">
-        <v>0.06562891</v>
+        <v>0.063999040000000007</v>
       </c>
       <c r="O22" s="277" t="s">
         <v>196</v>
@@ -68305,16 +68305,16 @@
         <v>75</v>
       </c>
       <c r="K23" s="274">
-        <v>2.80619056</v>
+        <v>2.8083035</v>
       </c>
       <c r="L23" s="274">
-        <v>-1.144E-05</v>
+        <v>-1.2630000000000001E-05</v>
       </c>
       <c r="M23" s="274">
-        <v>0.7841560500000001</v>
+        <v>0.78432642999999991</v>
       </c>
       <c r="N23" s="274">
-        <v>-0.55751156</v>
+        <v>-0.55962534</v>
       </c>
       <c r="O23" s="277" t="s">
         <v>199</v>
@@ -68368,16 +68368,16 @@
         <v>75</v>
       </c>
       <c r="K25" s="274">
-        <v>2.54706709</v>
+        <v>2.5478175</v>
       </c>
       <c r="L25" s="274">
-        <v>-7.29E-05</v>
+        <v>-7.365E-05</v>
       </c>
       <c r="M25" s="274">
-        <v>0.79759422</v>
+        <v>0.69090329</v>
       </c>
       <c r="N25" s="274">
-        <v>-0.32220359000000004</v>
+        <v>-0.21615773000000002</v>
       </c>
       <c r="O25" s="277" t="s">
         <v>202</v>
@@ -68431,16 +68431,16 @@
         <v>75</v>
       </c>
       <c r="K27" s="274">
-        <v>2.82278317</v>
+        <v>2.82365259</v>
       </c>
       <c r="L27" s="274">
-        <v>0.095387969999999989</v>
+        <v>0.09574665</v>
       </c>
       <c r="M27" s="274">
-        <v>0.23299173</v>
+        <v>0.19325182000000002</v>
       </c>
       <c r="N27" s="274">
-        <v>-0.12362880999999999</v>
+        <v>-0.08525494</v>
       </c>
       <c r="O27" s="277" t="s">
         <v>205</v>
@@ -68475,16 +68475,16 @@
         <v>75</v>
       </c>
       <c r="K28" s="274">
-        <v>2.54706709</v>
+        <v>2.5478175</v>
       </c>
       <c r="L28" s="274">
-        <v>-7.29E-05</v>
+        <v>-7.365E-05</v>
       </c>
       <c r="M28" s="274">
-        <v>0.79759422</v>
+        <v>0.69090329</v>
       </c>
       <c r="N28" s="274">
-        <v>-0.32220359000000004</v>
+        <v>-0.21615773000000002</v>
       </c>
       <c r="O28" s="277" t="s">
         <v>202</v>
@@ -68538,16 +68538,16 @@
         <v>75</v>
       </c>
       <c r="K30" s="274">
-        <v>2.80619056</v>
+        <v>2.8083035</v>
       </c>
       <c r="L30" s="274">
-        <v>-1.144E-05</v>
+        <v>-1.2630000000000001E-05</v>
       </c>
       <c r="M30" s="274">
-        <v>0.7841560500000001</v>
+        <v>0.78432642999999991</v>
       </c>
       <c r="N30" s="274">
-        <v>-0.55751156</v>
+        <v>-0.55962534</v>
       </c>
       <c r="O30" s="277" t="s">
         <v>199</v>
@@ -68582,16 +68582,16 @@
         <v>75</v>
       </c>
       <c r="K31" s="274">
-        <v>2.80619056</v>
+        <v>2.8083035</v>
       </c>
       <c r="L31" s="274">
-        <v>-1.144E-05</v>
+        <v>-1.2630000000000001E-05</v>
       </c>
       <c r="M31" s="274">
-        <v>0.7841560500000001</v>
+        <v>0.78432642999999991</v>
       </c>
       <c r="N31" s="274">
-        <v>-0.55751156</v>
+        <v>-0.55962534</v>
       </c>
       <c r="O31" s="277" t="s">
         <v>199</v>
@@ -68626,16 +68626,16 @@
         <v>75</v>
       </c>
       <c r="K32" s="274">
-        <v>2.80619056</v>
+        <v>2.8083035</v>
       </c>
       <c r="L32" s="274">
-        <v>-1.144E-05</v>
+        <v>-1.2630000000000001E-05</v>
       </c>
       <c r="M32" s="274">
-        <v>0.7841560500000001</v>
+        <v>0.78432642999999991</v>
       </c>
       <c r="N32" s="274">
-        <v>-0.55751156</v>
+        <v>-0.55962534</v>
       </c>
       <c r="O32" s="277" t="s">
         <v>199</v>
@@ -68670,16 +68670,16 @@
         <v>75</v>
       </c>
       <c r="K33" s="274">
-        <v>2.50310454</v>
+        <v>2.50927331</v>
       </c>
       <c r="L33" s="274">
-        <v>4.66E-06</v>
+        <v>3.26E-06</v>
       </c>
       <c r="M33" s="274">
-        <v>0.3525406</v>
+        <v>0.35211265</v>
       </c>
       <c r="N33" s="274">
-        <v>0.16790042</v>
+        <v>0.15788451</v>
       </c>
       <c r="O33" s="277" t="s">
         <v>212</v>
@@ -68733,16 +68733,16 @@
         <v>75</v>
       </c>
       <c r="K35" s="274">
-        <v>2.5018627799999997</v>
+        <v>2.50203517</v>
       </c>
       <c r="L35" s="274">
-        <v>-0.00023595000000000002</v>
+        <v>1.793E-05</v>
       </c>
       <c r="M35" s="274">
-        <v>0.63809325000000006</v>
+        <v>0.64202115</v>
       </c>
       <c r="N35" s="274">
-        <v>-0.11834933</v>
+        <v>-0.12207063000000001</v>
       </c>
       <c r="O35" s="277" t="s">
         <v>215</v>
@@ -68777,16 +68777,16 @@
         <v>75</v>
       </c>
       <c r="K36" s="274">
-        <v>2.56819223</v>
+        <v>2.55356732</v>
       </c>
       <c r="L36" s="274">
-        <v>-4.88E-06</v>
+        <v>-4.097E-05</v>
       </c>
       <c r="M36" s="274">
-        <v>3.68762173</v>
+        <v>3.68483317</v>
       </c>
       <c r="N36" s="274">
-        <v>-3.22913731</v>
+        <v>-3.2142419700000002</v>
       </c>
       <c r="O36" s="277" t="s">
         <v>217</v>
@@ -68821,16 +68821,16 @@
         <v>75</v>
       </c>
       <c r="K37" s="274">
-        <v>2.50310454</v>
+        <v>2.50927331</v>
       </c>
       <c r="L37" s="274">
-        <v>4.66E-06</v>
+        <v>3.26E-06</v>
       </c>
       <c r="M37" s="274">
-        <v>0.3525406</v>
+        <v>0.35211265</v>
       </c>
       <c r="N37" s="274">
-        <v>0.16790042</v>
+        <v>0.15788451</v>
       </c>
       <c r="O37" s="277" t="s">
         <v>212</v>
@@ -68884,16 +68884,16 @@
         <v>6</v>
       </c>
       <c r="K39" s="274">
-        <v>2.47908301</v>
+        <v>2.4852945</v>
       </c>
       <c r="L39" s="274">
-        <v>9.05E-06</v>
+        <v>8.36E-06</v>
       </c>
       <c r="M39" s="274">
-        <v>0.35250947</v>
+        <v>0.35193019000000003</v>
       </c>
       <c r="N39" s="274">
-        <v>0.19301190000000001</v>
+        <v>0.18185241</v>
       </c>
       <c r="O39" s="277" t="s">
         <v>221</v>
@@ -68928,16 +68928,16 @@
         <v>6</v>
       </c>
       <c r="K40" s="274">
-        <v>2.47908301</v>
+        <v>2.4852945</v>
       </c>
       <c r="L40" s="274">
-        <v>9.05E-06</v>
+        <v>8.36E-06</v>
       </c>
       <c r="M40" s="274">
-        <v>0.35250947</v>
+        <v>0.35193019000000003</v>
       </c>
       <c r="N40" s="274">
-        <v>0.19301190000000001</v>
+        <v>0.18185241</v>
       </c>
       <c r="O40" s="277" t="s">
         <v>221</v>
@@ -68972,16 +68972,16 @@
         <v>6</v>
       </c>
       <c r="K41" s="274">
-        <v>2.47908301</v>
+        <v>2.4852945</v>
       </c>
       <c r="L41" s="274">
-        <v>9.05E-06</v>
+        <v>8.36E-06</v>
       </c>
       <c r="M41" s="274">
-        <v>0.35250947</v>
+        <v>0.35193019000000003</v>
       </c>
       <c r="N41" s="274">
-        <v>0.19301190000000001</v>
+        <v>0.18185241</v>
       </c>
       <c r="O41" s="277" t="s">
         <v>221</v>
@@ -69425,7 +69425,7 @@
         <v>6</v>
       </c>
       <c r="K53" s="274">
-        <v>2.47869737</v>
+        <v>3.1154958600000002</v>
       </c>
       <c r="L53" s="274">
         <v>0</v>
@@ -69434,7 +69434,7 @@
         <v>0</v>
       </c>
       <c r="N53" s="274">
-        <v>0.58445916</v>
+        <v>-0.05249275</v>
       </c>
       <c r="O53" s="277" t="s">
         <v>242</v>
@@ -69648,7 +69648,7 @@
         <v>6</v>
       </c>
       <c r="Z6" s="0">
-        <v>5</v>
+        <v>0.0025</v>
       </c>
       <c r="AA6" s="0" t="s">
         <v>6</v>
@@ -69706,7 +69706,7 @@
         <v>6</v>
       </c>
       <c r="Z7" s="0">
-        <v>0.755208333333333</v>
+        <v>1.49479166666667</v>
       </c>
       <c r="AA7" s="0" t="s">
         <v>6</v>
@@ -69756,7 +69756,7 @@
         <v>6</v>
       </c>
       <c r="Z8" s="0">
-        <v>5</v>
+        <v>0.0025</v>
       </c>
       <c r="AA8" s="0" t="s">
         <v>6</v>
@@ -69806,7 +69806,7 @@
         <v>6</v>
       </c>
       <c r="Z9" s="0">
-        <v>10.125</v>
+        <v>10.375</v>
       </c>
       <c r="AA9" s="0" t="s">
         <v>6</v>
@@ -69856,7 +69856,7 @@
         <v>6</v>
       </c>
       <c r="Z10" s="0">
-        <v>10.125</v>
+        <v>10.375</v>
       </c>
       <c r="AA10" s="0" t="s">
         <v>6</v>
@@ -69906,7 +69906,7 @@
         <v>6</v>
       </c>
       <c r="Z11" s="0">
-        <v>0.4140625</v>
+        <v>5.47916666666667</v>
       </c>
       <c r="AA11" s="0" t="s">
         <v>6</v>
@@ -69956,7 +69956,7 @@
         <v>6</v>
       </c>
       <c r="Z12" s="0">
-        <v>10.125</v>
+        <v>10.375</v>
       </c>
       <c r="AA12" s="0" t="s">
         <v>6</v>
@@ -70010,7 +70010,7 @@
         <v>6</v>
       </c>
       <c r="Z13" s="0">
-        <v>14.0416666666667</v>
+        <v>14.125</v>
       </c>
       <c r="AA13" s="0" t="s">
         <v>6</v>
@@ -70072,7 +70072,7 @@
         <v>6</v>
       </c>
       <c r="Z14" s="0">
-        <v>0.239583333333333</v>
+        <v>3.50735940085</v>
       </c>
       <c r="AA14" s="0" t="s">
         <v>6</v>
@@ -70122,7 +70122,7 @@
         <v>6</v>
       </c>
       <c r="Z15" s="0">
-        <v>9.70833333333333</v>
+        <v>9.95833333333333</v>
       </c>
       <c r="AA15" s="0" t="s">
         <v>6</v>
@@ -70180,7 +70180,7 @@
         <v>6</v>
       </c>
       <c r="Z16" s="0">
-        <v>9.54166666666667</v>
+        <v>9.79166666666667</v>
       </c>
       <c r="AA16" s="0" t="s">
         <v>6</v>
@@ -70230,7 +70230,7 @@
         <v>6</v>
       </c>
       <c r="Z17" s="0">
-        <v>0.296875</v>
+        <v>3.04166666666667</v>
       </c>
       <c r="AA17" s="0" t="s">
         <v>6</v>
@@ -70284,7 +70284,7 @@
         <v>6</v>
       </c>
       <c r="Z18" s="0">
-        <v>0.328125</v>
+        <v>4.04166666666667</v>
       </c>
       <c r="AA18" s="0" t="s">
         <v>25</v>
@@ -70340,7 +70340,7 @@
         <v>6</v>
       </c>
       <c r="Z19" s="0">
-        <v>17.375</v>
+        <v>17.4583333333333</v>
       </c>
       <c r="AA19" s="0" t="s">
         <v>25</v>
@@ -70408,7 +70408,7 @@
         <v>6</v>
       </c>
       <c r="Z20" s="0">
-        <v>0.0104166666666667</v>
+        <v>4.5662384743</v>
       </c>
       <c r="AA20" s="0" t="s">
         <v>25</v>
@@ -70462,7 +70462,7 @@
         <v>6</v>
       </c>
       <c r="Z21" s="0">
-        <v>0.473958333333333</v>
+        <v>1.54166666666667</v>
       </c>
       <c r="AA21" s="0" t="s">
         <v>25</v>
@@ -70516,7 +70516,7 @@
         <v>6</v>
       </c>
       <c r="Z22" s="0">
-        <v>0.302083333333333</v>
+        <v>2.95833333333333</v>
       </c>
       <c r="AA22" s="0" t="s">
         <v>25</v>
@@ -70578,7 +70578,7 @@
         <v>6</v>
       </c>
       <c r="Z23" s="0">
-        <v>0.3046875</v>
+        <v>2.79166666666667</v>
       </c>
       <c r="AA23" s="0" t="s">
         <v>25</v>
@@ -70640,7 +70640,7 @@
         <v>6</v>
       </c>
       <c r="Z24" s="0">
-        <v>0.302083333333333</v>
+        <v>2.79166666666667</v>
       </c>
       <c r="AA24" s="0" t="s">
         <v>25</v>
@@ -70702,7 +70702,7 @@
         <v>6</v>
       </c>
       <c r="Z25" s="0">
-        <v>0.307291666666667</v>
+        <v>2.79166666666667</v>
       </c>
       <c r="AA25" s="0" t="s">
         <v>25</v>
@@ -70764,7 +70764,7 @@
         <v>6</v>
       </c>
       <c r="Z26" s="0">
-        <v>0.3046875</v>
+        <v>2.79166666666667</v>
       </c>
       <c r="AA26" s="0" t="s">
         <v>25</v>
@@ -70818,7 +70818,7 @@
         <v>6</v>
       </c>
       <c r="Z27" s="0">
-        <v>16.4583333333333</v>
+        <v>16.5416666666667</v>
       </c>
       <c r="AA27" s="0" t="s">
         <v>25</v>
@@ -70872,7 +70872,7 @@
         <v>6</v>
       </c>
       <c r="Z28" s="0">
-        <v>8.79166666666667</v>
+        <v>8.875</v>
       </c>
       <c r="AA28" s="0" t="s">
         <v>25</v>
@@ -70934,7 +70934,7 @@
         <v>6</v>
       </c>
       <c r="Z29" s="0">
-        <v>8.625</v>
+        <v>8.70833333333333</v>
       </c>
       <c r="AA29" s="0" t="s">
         <v>25</v>
@@ -70996,7 +70996,7 @@
         <v>6</v>
       </c>
       <c r="Z30" s="0">
-        <v>8.625</v>
+        <v>8.70833333333333</v>
       </c>
       <c r="AA30" s="0" t="s">
         <v>25</v>
@@ -71058,7 +71058,7 @@
         <v>6</v>
       </c>
       <c r="Z31" s="0">
-        <v>8.54166666666667</v>
+        <v>8.625</v>
       </c>
       <c r="AA31" s="0" t="s">
         <v>25</v>
@@ -71120,7 +71120,7 @@
         <v>6</v>
       </c>
       <c r="Z32" s="0">
-        <v>8.5625</v>
+        <v>8.70833333333333</v>
       </c>
       <c r="AA32" s="0" t="s">
         <v>25</v>
@@ -71176,7 +71176,7 @@
         <v>6</v>
       </c>
       <c r="Z33" s="0">
-        <v>0.5625</v>
+        <v>1.71875</v>
       </c>
       <c r="AA33" s="0" t="s">
         <v>25</v>
@@ -71232,7 +71232,7 @@
         <v>6</v>
       </c>
       <c r="Z34" s="0">
-        <v>0.377604166666667</v>
+        <v>1.89583333333333</v>
       </c>
       <c r="AA34" s="0" t="s">
         <v>25</v>
@@ -71286,7 +71286,7 @@
         <v>6</v>
       </c>
       <c r="Z35" s="0">
-        <v>0.395833333333333</v>
+        <v>1.80208333333333</v>
       </c>
       <c r="AA35" s="0" t="s">
         <v>25</v>
@@ -71348,7 +71348,7 @@
         <v>6</v>
       </c>
       <c r="Z36" s="0">
-        <v>0.395833333333333</v>
+        <v>1.79166666666667</v>
       </c>
       <c r="AA36" s="0" t="s">
         <v>25</v>
@@ -71410,7 +71410,7 @@
         <v>6</v>
       </c>
       <c r="Z37" s="0">
-        <v>0.395833333333333</v>
+        <v>1.79166666666667</v>
       </c>
       <c r="AA37" s="0" t="s">
         <v>25</v>
@@ -71464,7 +71464,7 @@
         <v>6</v>
       </c>
       <c r="Z38" s="0">
-        <v>0.484375</v>
+        <v>0.463541666666667</v>
       </c>
       <c r="AA38" s="0" t="s">
         <v>25</v>
@@ -71526,7 +71526,7 @@
         <v>6</v>
       </c>
       <c r="Z39" s="0">
-        <v>0.486979166666667</v>
+        <v>0.46875</v>
       </c>
       <c r="AA39" s="0" t="s">
         <v>25</v>
@@ -71588,7 +71588,7 @@
         <v>6</v>
       </c>
       <c r="Z40" s="0">
-        <v>0.486979166666667</v>
+        <v>0.46875</v>
       </c>
       <c r="AA40" s="0" t="s">
         <v>25</v>
@@ -71642,7 +71642,7 @@
         <v>6</v>
       </c>
       <c r="Z41" s="0">
-        <v>0.380208333333333</v>
+        <v>4.95833333333333</v>
       </c>
       <c r="AA41" s="0" t="s">
         <v>25</v>
@@ -71704,7 +71704,7 @@
         <v>6</v>
       </c>
       <c r="Z42" s="0">
-        <v>0.377604166666667</v>
+        <v>4.95833333333333</v>
       </c>
       <c r="AA42" s="0" t="s">
         <v>25</v>
@@ -71766,7 +71766,7 @@
         <v>6</v>
       </c>
       <c r="Z43" s="0">
-        <v>0.380208333333333</v>
+        <v>4.95833333333333</v>
       </c>
       <c r="AA43" s="0" t="s">
         <v>25</v>
@@ -71828,7 +71828,7 @@
         <v>6</v>
       </c>
       <c r="Z44" s="0">
-        <v>0.377604166666667</v>
+        <v>4.95833333333333</v>
       </c>
       <c r="AA44" s="0" t="s">
         <v>25</v>
@@ -71890,7 +71890,7 @@
         <v>6</v>
       </c>
       <c r="Z45" s="0">
-        <v>0.380208333333333</v>
+        <v>4.95833333333333</v>
       </c>
       <c r="AA45" s="0" t="s">
         <v>25</v>
@@ -71946,7 +71946,7 @@
         <v>6</v>
       </c>
       <c r="Z46" s="0">
-        <v>16.4583333333333</v>
+        <v>16.5416666666667</v>
       </c>
       <c r="AA46" s="0" t="s">
         <v>25</v>
@@ -72002,7 +72002,7 @@
         <v>6</v>
       </c>
       <c r="Z47" s="0">
-        <v>8.79166666666667</v>
+        <v>8.875</v>
       </c>
       <c r="AA47" s="0" t="s">
         <v>25</v>
@@ -72066,7 +72066,7 @@
         <v>6</v>
       </c>
       <c r="Z48" s="0">
-        <v>8.625</v>
+        <v>8.70833333333333</v>
       </c>
       <c r="AA48" s="0" t="s">
         <v>25</v>
@@ -72130,7 +72130,7 @@
         <v>6</v>
       </c>
       <c r="Z49" s="0">
-        <v>8.625</v>
+        <v>8.70833333333333</v>
       </c>
       <c r="AA49" s="0" t="s">
         <v>25</v>
@@ -72194,7 +72194,7 @@
         <v>6</v>
       </c>
       <c r="Z50" s="0">
-        <v>8.54166666666667</v>
+        <v>8.625</v>
       </c>
       <c r="AA50" s="0" t="s">
         <v>25</v>
@@ -72258,7 +72258,7 @@
         <v>6</v>
       </c>
       <c r="Z51" s="0">
-        <v>8.5625</v>
+        <v>8.70833333333333</v>
       </c>
       <c r="AA51" s="0" t="s">
         <v>25</v>
@@ -72316,7 +72316,7 @@
         <v>6</v>
       </c>
       <c r="Z52" s="0">
-        <v>0.5625</v>
+        <v>1.71875</v>
       </c>
       <c r="AA52" s="0" t="s">
         <v>25</v>
@@ -72374,7 +72374,7 @@
         <v>6</v>
       </c>
       <c r="Z53" s="0">
-        <v>0.377604166666667</v>
+        <v>1.89583333333333</v>
       </c>
       <c r="AA53" s="0" t="s">
         <v>25</v>
@@ -72428,7 +72428,7 @@
         <v>6</v>
       </c>
       <c r="Z54" s="0">
-        <v>0.760416666666667</v>
+        <v>0.994791666666667</v>
       </c>
       <c r="AA54" s="0" t="s">
         <v>25</v>
@@ -72490,7 +72490,7 @@
         <v>6</v>
       </c>
       <c r="Z55" s="0">
-        <v>0.760416666666667</v>
+        <v>0.989583333333333</v>
       </c>
       <c r="AA55" s="0" t="s">
         <v>25</v>
@@ -72544,7 +72544,7 @@
         <v>6</v>
       </c>
       <c r="Z56" s="0">
-        <v>9.125</v>
+        <v>9.20833333333333</v>
       </c>
       <c r="AA56" s="0" t="s">
         <v>25</v>
@@ -72606,7 +72606,7 @@
         <v>6</v>
       </c>
       <c r="Z57" s="0">
-        <v>8.95833333333333</v>
+        <v>9.04166666666667</v>
       </c>
       <c r="AA57" s="0" t="s">
         <v>25</v>
@@ -72660,7 +72660,7 @@
         <v>6</v>
       </c>
       <c r="Z58" s="0">
-        <v>12.4583333333333</v>
+        <v>12.625</v>
       </c>
       <c r="AA58" s="0" t="s">
         <v>25</v>
@@ -72722,7 +72722,7 @@
         <v>6</v>
       </c>
       <c r="Z59" s="0">
-        <v>11.9583333333333</v>
+        <v>12.125</v>
       </c>
       <c r="AA59" s="0" t="s">
         <v>25</v>
@@ -72784,7 +72784,7 @@
         <v>6</v>
       </c>
       <c r="Z60" s="0">
-        <v>12.0416666666667</v>
+        <v>12.2083333333333</v>
       </c>
       <c r="AA60" s="0" t="s">
         <v>25</v>
@@ -72846,7 +72846,7 @@
         <v>6</v>
       </c>
       <c r="Z61" s="0">
-        <v>11.5416666666667</v>
+        <v>11.7083333333333</v>
       </c>
       <c r="AA61" s="0" t="s">
         <v>25</v>
@@ -72908,7 +72908,7 @@
         <v>6</v>
       </c>
       <c r="Z62" s="0">
-        <v>11.9583333333333</v>
+        <v>12.125</v>
       </c>
       <c r="AA62" s="0" t="s">
         <v>25</v>
@@ -72962,7 +72962,7 @@
         <v>6</v>
       </c>
       <c r="Z63" s="0">
-        <v>0.299479166666667</v>
+        <v>2.95833333333333</v>
       </c>
       <c r="AA63" s="0" t="s">
         <v>25</v>
@@ -73024,7 +73024,7 @@
         <v>6</v>
       </c>
       <c r="Z64" s="0">
-        <v>0.302083333333333</v>
+        <v>2.95833333333333</v>
       </c>
       <c r="AA64" s="0" t="s">
         <v>25</v>
@@ -73086,7 +73086,7 @@
         <v>6</v>
       </c>
       <c r="Z65" s="0">
-        <v>0.302083333333333</v>
+        <v>2.95833333333333</v>
       </c>
       <c r="AA65" s="0" t="s">
         <v>25</v>
@@ -73148,7 +73148,7 @@
         <v>6</v>
       </c>
       <c r="Z66" s="0">
-        <v>0.302083333333333</v>
+        <v>3.04166666666667</v>
       </c>
       <c r="AA66" s="0" t="s">
         <v>25</v>
@@ -73210,7 +73210,7 @@
         <v>6</v>
       </c>
       <c r="Z67" s="0">
-        <v>0.302083333333333</v>
+        <v>2.95833333333333</v>
       </c>
       <c r="AA67" s="0" t="s">
         <v>25</v>
@@ -73264,7 +73264,7 @@
         <v>6</v>
       </c>
       <c r="Z68" s="0">
-        <v>0.375</v>
+        <v>1.85416666666667</v>
       </c>
       <c r="AA68" s="0" t="s">
         <v>25</v>
@@ -73318,7 +73318,7 @@
         <v>6</v>
       </c>
       <c r="Z69" s="0">
-        <v>0.375</v>
+        <v>1.85416666666667</v>
       </c>
       <c r="AA69" s="0" t="s">
         <v>25</v>
@@ -73372,7 +73372,7 @@
         <v>6</v>
       </c>
       <c r="Z70" s="0">
-        <v>0.375</v>
+        <v>1.85416666666667</v>
       </c>
       <c r="AA70" s="0" t="s">
         <v>25</v>
@@ -73426,7 +73426,7 @@
         <v>6</v>
       </c>
       <c r="Z71" s="0">
-        <v>0.375</v>
+        <v>1.85416666666667</v>
       </c>
       <c r="AA71" s="0" t="s">
         <v>25</v>
@@ -73480,7 +73480,7 @@
         <v>6</v>
       </c>
       <c r="Z72" s="0">
-        <v>0.375</v>
+        <v>1.85416666666667</v>
       </c>
       <c r="AA72" s="0" t="s">
         <v>25</v>
@@ -73534,7 +73534,7 @@
         <v>6</v>
       </c>
       <c r="Z73" s="0">
-        <v>0.375</v>
+        <v>1.85416666666667</v>
       </c>
       <c r="AA73" s="0" t="s">
         <v>25</v>
@@ -73588,7 +73588,7 @@
         <v>6</v>
       </c>
       <c r="Z74" s="0">
-        <v>0.375</v>
+        <v>1.85416666666667</v>
       </c>
       <c r="AA74" s="0" t="s">
         <v>25</v>
@@ -73642,7 +73642,7 @@
         <v>6</v>
       </c>
       <c r="Z75" s="0">
-        <v>0.375</v>
+        <v>1.85416666666667</v>
       </c>
       <c r="AA75" s="0" t="s">
         <v>25</v>
@@ -73696,7 +73696,7 @@
         <v>6</v>
       </c>
       <c r="Z76" s="0">
-        <v>0.369791666666667</v>
+        <v>1.875</v>
       </c>
       <c r="AA76" s="0" t="s">
         <v>25</v>
@@ -73750,7 +73750,7 @@
         <v>6</v>
       </c>
       <c r="Z77" s="0">
-        <v>0.369791666666667</v>
+        <v>1.875</v>
       </c>
       <c r="AA77" s="0" t="s">
         <v>25</v>
@@ -73804,7 +73804,7 @@
         <v>6</v>
       </c>
       <c r="Z78" s="0">
-        <v>0.359375</v>
+        <v>1.89583333333333</v>
       </c>
       <c r="AA78" s="0" t="s">
         <v>25</v>
@@ -73858,7 +73858,7 @@
         <v>6</v>
       </c>
       <c r="Z79" s="0">
-        <v>0.359375</v>
+        <v>1.89583333333333</v>
       </c>
       <c r="AA79" s="0" t="s">
         <v>25</v>
@@ -73912,7 +73912,7 @@
         <v>6</v>
       </c>
       <c r="Z80" s="0">
-        <v>0.497395833333333</v>
+        <v>6.29166666666667</v>
       </c>
       <c r="AA80" s="0" t="s">
         <v>25</v>
@@ -73966,7 +73966,7 @@
         <v>6</v>
       </c>
       <c r="Z81" s="0">
-        <v>0.572916666666667</v>
+        <v>0.489583333333333</v>
       </c>
       <c r="AA81" s="0" t="s">
         <v>25</v>
@@ -74020,7 +74020,7 @@
         <v>6</v>
       </c>
       <c r="Z82" s="0">
-        <v>0.572916666666667</v>
+        <v>0.484375</v>
       </c>
       <c r="AA82" s="0" t="s">
         <v>25</v>
@@ -74074,7 +74074,7 @@
         <v>6</v>
       </c>
       <c r="Z83" s="0">
-        <v>0.5625</v>
+        <v>1.53125</v>
       </c>
       <c r="AA83" s="0" t="s">
         <v>25</v>
@@ -74128,7 +74128,7 @@
         <v>6</v>
       </c>
       <c r="Z84" s="0">
-        <v>0.484375</v>
+        <v>0.463541666666667</v>
       </c>
       <c r="AA84" s="0" t="s">
         <v>25</v>
@@ -74190,7 +74190,7 @@
         <v>6</v>
       </c>
       <c r="Z85" s="0">
-        <v>0.484375</v>
+        <v>0.466145833333333</v>
       </c>
       <c r="AA85" s="0" t="s">
         <v>25</v>
@@ -74244,7 +74244,7 @@
         <v>6</v>
       </c>
       <c r="Z86" s="0">
-        <v>0.328125</v>
+        <v>4.04166666666667</v>
       </c>
       <c r="AA86" s="0" t="s">
         <v>25</v>
@@ -74294,7 +74294,7 @@
         <v>6</v>
       </c>
       <c r="Z87" s="0">
-        <v>0.328125</v>
+        <v>4.04166666666667</v>
       </c>
       <c r="AA87" s="0" t="s">
         <v>6</v>
@@ -74344,7 +74344,7 @@
         <v>6</v>
       </c>
       <c r="Z88" s="0">
-        <v>0.328125</v>
+        <v>4.04166666666667</v>
       </c>
       <c r="AA88" s="0" t="s">
         <v>6</v>
@@ -74394,7 +74394,7 @@
         <v>6</v>
       </c>
       <c r="Z89" s="0">
-        <v>5</v>
+        <v>0.0025</v>
       </c>
       <c r="AA89" s="0" t="s">
         <v>6</v>
@@ -74444,7 +74444,7 @@
         <v>6</v>
       </c>
       <c r="Z90" s="0">
-        <v>19.9583333333333</v>
+        <v>2.6980874526</v>
       </c>
       <c r="AA90" s="0" t="s">
         <v>6</v>
@@ -74494,7 +74494,7 @@
         <v>6</v>
       </c>
       <c r="Z91" s="0">
-        <v>20.375</v>
+        <v>13.9826805052</v>
       </c>
       <c r="AA91" s="0" t="s">
         <v>6</v>
@@ -74544,7 +74544,7 @@
         <v>6</v>
       </c>
       <c r="Z92" s="0">
-        <v>18.625</v>
+        <v>11.077893223</v>
       </c>
       <c r="AA92" s="0" t="s">
         <v>6</v>
@@ -74594,7 +74594,7 @@
         <v>6</v>
       </c>
       <c r="Z93" s="0">
-        <v>17.375</v>
+        <v>8.2248232356</v>
       </c>
       <c r="AA93" s="0" t="s">
         <v>6</v>
@@ -74644,7 +74644,7 @@
         <v>6</v>
       </c>
       <c r="Z94" s="0">
-        <v>18.375</v>
+        <v>5.4341142672</v>
       </c>
       <c r="AA94" s="0" t="s">
         <v>6</v>
@@ -74694,7 +74694,7 @@
         <v>6</v>
       </c>
       <c r="Z95" s="0">
-        <v>19.9583333333333</v>
+        <v>2.6980874526</v>
       </c>
       <c r="AA95" s="0" t="s">
         <v>6</v>
@@ -74744,7 +74744,7 @@
         <v>6</v>
       </c>
       <c r="Z96" s="0">
-        <v>17.125</v>
+        <v>1.330998303</v>
       </c>
       <c r="AA96" s="0" t="s">
         <v>6</v>
@@ -74794,7 +74794,7 @@
         <v>6</v>
       </c>
       <c r="Z97" s="0">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="AA97" s="0" t="s">
         <v>6</v>
@@ -74844,7 +74844,7 @@
         <v>6</v>
       </c>
       <c r="Z98" s="0">
-        <v>18.0416666666667</v>
+        <v>10</v>
       </c>
       <c r="AA98" s="0" t="s">
         <v>6</v>
@@ -74894,7 +74894,7 @@
         <v>6</v>
       </c>
       <c r="Z99" s="0">
-        <v>16.4583333333333</v>
+        <v>8</v>
       </c>
       <c r="AA99" s="0" t="s">
         <v>6</v>
@@ -74944,7 +74944,7 @@
         <v>6</v>
       </c>
       <c r="Z100" s="0">
-        <v>15.375</v>
+        <v>6</v>
       </c>
       <c r="AA100" s="0" t="s">
         <v>6</v>
@@ -74994,7 +74994,7 @@
         <v>6</v>
       </c>
       <c r="Z101" s="0">
-        <v>18.2083333333333</v>
+        <v>4.0000149712</v>
       </c>
       <c r="AA101" s="0" t="s">
         <v>6</v>
@@ -75044,7 +75044,7 @@
         <v>6</v>
       </c>
       <c r="Z102" s="0">
-        <v>24.7916666666667</v>
+        <v>2</v>
       </c>
       <c r="AA102" s="0" t="s">
         <v>6</v>
@@ -75094,7 +75094,7 @@
         <v>6</v>
       </c>
       <c r="Z103" s="0">
-        <v>16.125</v>
+        <v>1</v>
       </c>
       <c r="AA103" s="0" t="s">
         <v>6</v>
@@ -75144,7 +75144,7 @@
         <v>6</v>
       </c>
       <c r="Z104" s="0">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="AA104" s="0" t="s">
         <v>6</v>
@@ -75194,7 +75194,7 @@
         <v>6</v>
       </c>
       <c r="Z105" s="0">
-        <v>5</v>
+        <v>5.4340042562</v>
       </c>
       <c r="AA105" s="0" t="s">
         <v>6</v>
@@ -75244,7 +75244,7 @@
         <v>6</v>
       </c>
       <c r="Z106" s="0">
-        <v>9.70833333333333</v>
+        <v>10.2916666666667</v>
       </c>
       <c r="AA106" s="0" t="s">
         <v>6</v>
@@ -75294,7 +75294,7 @@
         <v>6</v>
       </c>
       <c r="Z107" s="0">
-        <v>0.65625</v>
+        <v>7.04166666666667</v>
       </c>
       <c r="AA107" s="0" t="s">
         <v>6</v>
@@ -75344,7 +75344,7 @@
         <v>6</v>
       </c>
       <c r="Z108" s="0">
-        <v>0.380208333333333</v>
+        <v>5.01041666666667</v>
       </c>
       <c r="AA108" s="0" t="s">
         <v>6</v>
@@ -75394,7 +75394,7 @@
         <v>6</v>
       </c>
       <c r="Z109" s="0">
-        <v>0.299479166666667</v>
+        <v>3.02083333333333</v>
       </c>
       <c r="AA109" s="0" t="s">
         <v>6</v>
@@ -75444,7 +75444,7 @@
         <v>6</v>
       </c>
       <c r="Z110" s="0">
-        <v>0.770833333333333</v>
+        <v>0.958333333333333</v>
       </c>
       <c r="AA110" s="0" t="s">
         <v>6</v>
@@ -75494,7 +75494,7 @@
         <v>6</v>
       </c>
       <c r="Z111" s="0">
-        <v>5</v>
+        <v>0.0729166666666667</v>
       </c>
       <c r="AA111" s="0" t="s">
         <v>6</v>
@@ -75552,7 +75552,7 @@
         <v>6</v>
       </c>
       <c r="Z112" s="0">
-        <v>0.770833333333333</v>
+        <v>0.994791666666667</v>
       </c>
       <c r="AA112" s="0" t="s">
         <v>6</v>
@@ -75602,7 +75602,7 @@
         <v>6</v>
       </c>
       <c r="Z113" s="0">
-        <v>0.328125</v>
+        <v>4.02083333333333</v>
       </c>
       <c r="AA113" s="0" t="s">
         <v>6</v>
@@ -75652,7 +75652,7 @@
         <v>6</v>
       </c>
       <c r="Z114" s="0">
-        <v>5</v>
+        <v>0.0025</v>
       </c>
       <c r="AA114" s="0" t="s">
         <v>6</v>

</xml_diff>